<commit_message>
update : modify data.xlsx for improved data handling
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -436,9 +436,26 @@
         <v>5689564556</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>test</v>
+      </c>
+      <c r="B3" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="C3" t="str">
+        <v>32442</v>
+      </c>
+      <c r="D3" t="str">
+        <v>indore</v>
+      </c>
+      <c r="E3" t="str">
+        <v>9656005657</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add : implement Excel file upload handling and data processing with multer
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -418,44 +418,154 @@
       <c r="E1" t="str">
         <v>Number</v>
       </c>
+      <c r="F1" t="str">
+        <v>Amount</v>
+      </c>
+      <c r="G1" t="str">
+        <v>UserId</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>sonuji</v>
+        <v>RETHEESH R</v>
       </c>
       <c r="B2" t="str">
-        <v>sonuji.ranju@gmail.com</v>
+        <v xml:space="preserve"> rrmulayara@gmail.com</v>
       </c>
       <c r="C2" t="str">
-        <v>ALCHP-INS-20251547873</v>
+        <v>ALCHP-INS-202509987</v>
       </c>
       <c r="D2" t="str">
-        <v>Revathy House, Irinjalakuda, Thrissur, Kerala, 680121</v>
+        <v xml:space="preserve"> rrmulayara@gmail.com</v>
       </c>
       <c r="E2" t="str">
-        <v>5689564556</v>
+        <v>ALCHP-INS-202509987</v>
+      </c>
+      <c r="F2">
+        <v>25023</v>
+      </c>
+      <c r="G2" t="str">
+        <v>CROWN-109987</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>test</v>
+        <v>Ranju Kanat</v>
       </c>
       <c r="B3" t="str">
-        <v>test@t.com</v>
+        <v>menonranju777@gmail.com</v>
       </c>
       <c r="C3" t="str">
-        <v>32442</v>
+        <v>ALCHP-INS-202513805</v>
       </c>
       <c r="D3" t="str">
-        <v>indore</v>
+        <v>menonranju777@gmail.com</v>
       </c>
       <c r="E3" t="str">
-        <v>9656005657</v>
+        <v>ALCHP-INS-202513805</v>
+      </c>
+      <c r="F3">
+        <v>26234</v>
+      </c>
+      <c r="G3" t="str">
+        <v>CROWN-113805</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Padma Priya</v>
+      </c>
+      <c r="B4" t="str">
+        <v>padmapriya.ranju@gmail.com</v>
+      </c>
+      <c r="C4" t="str">
+        <v>ALCHP-INS-202514173</v>
+      </c>
+      <c r="D4" t="str">
+        <v>padmapriya.ranju@gmail.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>ALCHP-INS-202514173</v>
+      </c>
+      <c r="F4">
+        <v>20010</v>
+      </c>
+      <c r="G4" t="str">
+        <v>CROWN-114173</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Srikanth</v>
+      </c>
+      <c r="B5" t="str">
+        <v>menonranju777@gmail.com</v>
+      </c>
+      <c r="C5" t="str">
+        <v>ALCHP-INS-202514734</v>
+      </c>
+      <c r="D5" t="str">
+        <v>menonranju777@gmail.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>ALCHP-INS-202514734</v>
+      </c>
+      <c r="F5">
+        <v>28025</v>
+      </c>
+      <c r="G5" t="str">
+        <v>CROWN-114734</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">Abraham </v>
+      </c>
+      <c r="B6" t="str">
+        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
+      </c>
+      <c r="C6" t="str">
+        <v>ALCHP-INS-202512447</v>
+      </c>
+      <c r="D6" t="str">
+        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
+      </c>
+      <c r="E6" t="str">
+        <v>ALCHP-INS-202512447</v>
+      </c>
+      <c r="F6">
+        <v>26212</v>
+      </c>
+      <c r="G6" t="str">
+        <v>CROWN-112447</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Ally</v>
+      </c>
+      <c r="B7" t="str">
+        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
+      </c>
+      <c r="C7" t="str">
+        <v>ALCHP-INS-202513061</v>
+      </c>
+      <c r="D7" t="str">
+        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
+      </c>
+      <c r="E7" t="str">
+        <v>ALCHP-INS-202513061</v>
+      </c>
+      <c r="F7">
+        <v>26230</v>
+      </c>
+      <c r="G7" t="str">
+        <v>CROWN-113061</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add : implement Excel file upload and processing functionality
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -32,8 +32,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -64,8 +65,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,175 +399,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>Name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>Email</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>InsuranceNumber</v>
       </c>
-      <c r="D1" t="str">
+      <c r="D1" s="1" t="str">
         <v>Address</v>
       </c>
-      <c r="E1" t="str">
+      <c r="E1" s="1" t="str">
         <v>Number</v>
       </c>
-      <c r="F1" t="str">
+      <c r="F1" s="1" t="str">
         <v>Amount</v>
       </c>
-      <c r="G1" t="str">
+      <c r="G1" s="1" t="str">
         <v>UserId</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>RETHEESH R</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="1" t="str">
         <v xml:space="preserve"> rrmulayara@gmail.com</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="1" t="str">
         <v>ALCHP-INS-202509987</v>
       </c>
-      <c r="D2" t="str">
-        <v xml:space="preserve"> rrmulayara@gmail.com</v>
-      </c>
-      <c r="E2" t="str">
-        <v>ALCHP-INS-202509987</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1" t="str">
+        <v>Karunya, Ambancode, Peyad PO, Trivandrum, Kerala, INDIA, Pincode: 695573</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9656005657</v>
+      </c>
+      <c r="F2" s="1">
         <v>25023</v>
       </c>
-      <c r="G2" t="str">
+      <c r="G2" s="1" t="str">
         <v>CROWN-109987</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Ranju Kanat</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="1" t="str">
         <v>menonranju777@gmail.com</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="1" t="str">
         <v>ALCHP-INS-202513805</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D3" s="1" t="str">
+        <v>Revathy House, Ayyankavu Temple Road, Irinjalakuda, Thrissur, Pincode: 680121</v>
+      </c>
+      <c r="E3" s="1">
+        <v>8075937035</v>
+      </c>
+      <c r="F3" s="1">
+        <v>26234</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <v>CROWN-113805</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>Padma Priya</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <v>padmapriya.ranju@gmail.com</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <v>ALCHP-INS-202514173</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <v>Revathy House, Ayyankavu Temple Road, Irinjalakuda, Thrissur, Pincode: 680121</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9496143678</v>
+      </c>
+      <c r="F4" s="1">
+        <v>20010</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <v>CROWN-114173</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>Srikanth</v>
+      </c>
+      <c r="B5" s="1" t="str">
         <v>menonranju777@gmail.com</v>
       </c>
-      <c r="E3" t="str">
-        <v>ALCHP-INS-202513805</v>
-      </c>
-      <c r="F3">
-        <v>26234</v>
-      </c>
-      <c r="G3" t="str">
-        <v>CROWN-113805</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Padma Priya</v>
-      </c>
-      <c r="B4" t="str">
-        <v>padmapriya.ranju@gmail.com</v>
-      </c>
-      <c r="C4" t="str">
-        <v>ALCHP-INS-202514173</v>
-      </c>
-      <c r="D4" t="str">
-        <v>padmapriya.ranju@gmail.com</v>
-      </c>
-      <c r="E4" t="str">
-        <v>ALCHP-INS-202514173</v>
-      </c>
-      <c r="F4">
-        <v>20010</v>
-      </c>
-      <c r="G4" t="str">
-        <v>CROWN-114173</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Srikanth</v>
-      </c>
-      <c r="B5" t="str">
-        <v>menonranju777@gmail.com</v>
-      </c>
-      <c r="C5" t="str">
+      <c r="C5" s="1" t="str">
         <v>ALCHP-INS-202514734</v>
       </c>
-      <c r="D5" t="str">
-        <v>menonranju777@gmail.com</v>
-      </c>
-      <c r="E5" t="str">
-        <v>ALCHP-INS-202514734</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="1" t="str">
+        <v>Revathy House, Ayyankavu Temple Road, Irinjalakuda, Thrissur, Pincode: 680121</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9496143678</v>
+      </c>
+      <c r="F5" s="1">
         <v>28025</v>
       </c>
-      <c r="G5" t="str">
+      <c r="G5" s="1" t="str">
         <v>CROWN-114734</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v xml:space="preserve">Abraham </v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="1" t="str">
         <v xml:space="preserve">ebrothekkekara@gmail.com </v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="1" t="str">
         <v>ALCHP-INS-202512447</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D6" s="1" t="str">
+        <v xml:space="preserve">Thekkekara House,Chettiparambu, Irinjalakuda, Thrissur District, Kerala, India </v>
+      </c>
+      <c r="E6" s="1">
+        <v>9946580236</v>
+      </c>
+      <c r="F6" s="1">
+        <v>26212</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <v>CROWN-112447</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>Ally</v>
+      </c>
+      <c r="B7" s="1" t="str">
         <v xml:space="preserve">ebrothekkekara@gmail.com </v>
       </c>
-      <c r="E6" t="str">
-        <v>ALCHP-INS-202512447</v>
-      </c>
-      <c r="F6">
-        <v>26212</v>
-      </c>
-      <c r="G6" t="str">
-        <v>CROWN-112447</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Ally</v>
-      </c>
-      <c r="B7" t="str">
-        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
-      </c>
-      <c r="C7" t="str">
+      <c r="C7" s="1" t="str">
         <v>ALCHP-INS-202513061</v>
       </c>
-      <c r="D7" t="str">
-        <v xml:space="preserve">ebrothekkekara@gmail.com </v>
-      </c>
-      <c r="E7" t="str">
-        <v>ALCHP-INS-202513061</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1" t="str">
+        <v xml:space="preserve">Thekkekara House,Chettiparambu, Irinjalakuda, Thrissur District, Kerala, India </v>
+      </c>
+      <c r="E7" s="1">
+        <v>9946580235</v>
+      </c>
+      <c r="F7" s="1">
         <v>26230</v>
       </c>
-      <c r="G7" t="str">
+      <c r="G7" s="1" t="str">
         <v>CROWN-113061</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>SMIJO</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <v>cleverladyiam@gmail.com</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <v>ALCHP-INS-202514445</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <v>Joby Chirayath House, Pazhuvil PO, Pin 680564, Thrissur</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7356140066</v>
+      </c>
+      <c r="F8" s="1">
+        <v>20025</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <v>CROWN-114445</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>